<commit_message>
going to make big big changes to ccopars
</commit_message>
<xml_diff>
--- a/tests/testprogramdata.xlsx
+++ b/tests/testprogramdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="28560" windowHeight="16980" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -254,9 +254,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -271,6 +268,9 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -587,15 +587,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="9"/>
+      <c r="A2" s="14"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="9"/>
+      <c r="A3" s="14"/>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1"/>
@@ -633,7 +633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -941,7 +941,7 @@
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
-      <c r="R3" s="10">
+      <c r="R3" s="9">
         <v>13000000</v>
       </c>
       <c r="S3" s="6"/>
@@ -974,10 +974,12 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+      <c r="O4" s="5">
+        <v>4</v>
+      </c>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="14">
+      <c r="R4" s="13">
         <v>5</v>
       </c>
       <c r="S4" s="5"/>
@@ -1013,7 +1015,7 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
-      <c r="R5" s="12">
+      <c r="R5" s="11">
         <f>R3/R4</f>
         <v>2600000</v>
       </c>
@@ -1048,13 +1050,15 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
+      <c r="P6" s="10">
+        <v>0.6</v>
+      </c>
       <c r="Q6" s="8"/>
-      <c r="R6" s="11">
+      <c r="R6" s="10"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="10">
         <v>0.75</v>
       </c>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
       <c r="W6" s="8"/>
@@ -1086,7 +1090,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
-      <c r="R8" s="10">
+      <c r="R8" s="9">
         <f>2500000</f>
         <v>2500000</v>
       </c>
@@ -1123,7 +1127,7 @@
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
-      <c r="R9" s="13">
+      <c r="R9" s="12">
         <v>30</v>
       </c>
       <c r="S9" s="5"/>
@@ -1159,7 +1163,7 @@
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
-      <c r="R10" s="12">
+      <c r="R10" s="11">
         <f>R8/R9</f>
         <v>83333.333333333328</v>
       </c>
@@ -1196,7 +1200,7 @@
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
-      <c r="R11" s="11">
+      <c r="R11" s="10">
         <v>0.9</v>
       </c>
       <c r="S11" s="8"/>
@@ -1232,7 +1236,7 @@
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
-      <c r="R13" s="10">
+      <c r="R13" s="9">
         <f>10000000</f>
         <v>10000000</v>
       </c>
@@ -1269,7 +1273,7 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
-      <c r="R14" s="13">
+      <c r="R14" s="12">
         <v>7.5</v>
       </c>
       <c r="S14" s="5"/>
@@ -1305,7 +1309,7 @@
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
-      <c r="R15" s="12">
+      <c r="R15" s="11">
         <f>R13/R14</f>
         <v>1333333.3333333333</v>
       </c>
@@ -1342,7 +1346,7 @@
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
-      <c r="R16" s="11">
+      <c r="R16" s="10">
         <v>0.9</v>
       </c>
       <c r="S16" s="8"/>
@@ -1378,7 +1382,7 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
-      <c r="R18" s="10">
+      <c r="R18" s="9">
         <f>20000000</f>
         <v>20000000</v>
       </c>
@@ -1415,7 +1419,7 @@
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
-      <c r="R19" s="13">
+      <c r="R19" s="12">
         <v>600</v>
       </c>
       <c r="S19" s="5"/>
@@ -1451,7 +1455,7 @@
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
-      <c r="R20" s="12">
+      <c r="R20" s="11">
         <f>R18/R19</f>
         <v>33333.333333333336</v>
       </c>
@@ -1488,7 +1492,7 @@
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
-      <c r="R21" s="11">
+      <c r="R21" s="10">
         <v>1</v>
       </c>
       <c r="S21" s="8"/>
@@ -1524,7 +1528,7 @@
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
-      <c r="R23" s="10">
+      <c r="R23" s="9">
         <f>15000000</f>
         <v>15000000</v>
       </c>

</xml_diff>

<commit_message>
actually not sure if this is simpler
</commit_message>
<xml_diff>
--- a/tests/testprogramdata.xlsx
+++ b/tests/testprogramdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="24940" windowHeight="13400" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="32">
   <si>
     <t>O P T I M A   2 . 0</t>
   </si>
@@ -98,13 +98,25 @@
     <t>OR</t>
   </si>
   <si>
-    <t>Unit cost</t>
-  </si>
-  <si>
-    <t>Coverage (optional)</t>
-  </si>
-  <si>
-    <t>Saturation (optional)</t>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>Unit cost - best</t>
+  </si>
+  <si>
+    <t>Unit cost - low</t>
+  </si>
+  <si>
+    <t>Unit cost - high</t>
+  </si>
+  <si>
+    <t>Saturation - best</t>
+  </si>
+  <si>
+    <t>Saturation - low</t>
+  </si>
+  <si>
+    <t>Saturation - high</t>
   </si>
 </sst>
 </file>
@@ -115,7 +127,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +169,14 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -230,7 +250,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -257,20 +277,26 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="43" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="43" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -587,15 +613,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="14"/>
+      <c r="A2" s="15"/>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="14"/>
+      <c r="A3" s="15"/>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1"/>
@@ -633,9 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -688,16 +712,16 @@
         <v>13</v>
       </c>
       <c r="E3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="5">
         <v>1</v>
@@ -834,16 +858,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="18" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -924,7 +948,7 @@
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Condoms</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="6"/>
@@ -960,8 +984,8 @@
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Condoms</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>25</v>
+      <c r="C4" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -974,17 +998,17 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
-      <c r="O4" s="5">
-        <v>4</v>
-      </c>
+      <c r="O4" s="10"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
-      <c r="R4" s="13">
+      <c r="R4" s="10">
         <v>5</v>
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
+      <c r="U4" s="13">
+        <v>7</v>
+      </c>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
@@ -998,8 +1022,8 @@
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Condoms</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>26</v>
+      <c r="C5" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -1012,16 +1036,15 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
+      <c r="O5" s="14"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
-      <c r="R5" s="11">
-        <f>R3/R4</f>
-        <v>2600000</v>
-      </c>
+      <c r="R5" s="8"/>
       <c r="S5" s="8"/>
       <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
+      <c r="U5" s="14">
+        <v>6</v>
+      </c>
       <c r="V5" s="8"/>
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
@@ -1035,8 +1058,8 @@
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Condoms</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>27</v>
+      <c r="C6" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -1049,17 +1072,15 @@
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="10">
-        <v>0.6</v>
-      </c>
+      <c r="O6" s="14"/>
+      <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
-      <c r="R6" s="10"/>
+      <c r="R6" s="8"/>
       <c r="S6" s="8"/>
-      <c r="T6" s="10">
-        <v>0.75</v>
-      </c>
-      <c r="U6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="14">
+        <v>8</v>
+      </c>
       <c r="V6" s="8"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
@@ -1068,86 +1089,122 @@
       </c>
       <c r="Z6" s="8"/>
     </row>
+    <row r="7" spans="1:26">
+      <c r="B7" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>Condoms</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="11">
+        <f>R3/R4</f>
+        <v>2600000</v>
+      </c>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z7" s="8"/>
+    </row>
     <row r="8" spans="1:26">
       <c r="B8" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
-        <v>FSW programs</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="9">
-        <f>2500000</f>
-        <v>2500000</v>
-      </c>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>Condoms</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
       <c r="Y8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z8" s="6"/>
+      <c r="Z8" s="8"/>
     </row>
     <row r="9" spans="1:26">
       <c r="B9" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
-        <v>FSW programs</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="12">
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>Condoms</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
       <c r="Y9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z9" s="5"/>
+      <c r="Z9" s="8"/>
     </row>
     <row r="10" spans="1:26">
       <c r="B10" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$4</f>
-        <v>FSW programs</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>26</v>
+        <f>'Populations &amp; programs'!$C$3</f>
+        <v>Condoms</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -1163,10 +1220,7 @@
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
-      <c r="R10" s="11">
-        <f>R8/R9</f>
-        <v>83333.333333333328</v>
-      </c>
+      <c r="R10" s="8"/>
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8"/>
@@ -1178,122 +1232,120 @@
       </c>
       <c r="Z10" s="8"/>
     </row>
-    <row r="11" spans="1:26">
-      <c r="B11" s="4" t="str">
+    <row r="12" spans="1:26">
+      <c r="B12" s="4" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>FSW programs</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z11" s="8"/>
+      <c r="C12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="9">
+        <f>2500000</f>
+        <v>2500000</v>
+      </c>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z12" s="6"/>
     </row>
     <row r="13" spans="1:26">
       <c r="B13" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
-        <v>HTC</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="9">
-        <f>10000000</f>
-        <v>10000000</v>
-      </c>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>FSW programs</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="13">
+        <v>30</v>
+      </c>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
       <c r="Y13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z13" s="6"/>
+      <c r="Z13" s="5"/>
     </row>
     <row r="14" spans="1:26">
       <c r="B14" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
-        <v>HTC</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="12">
-        <v>7.5</v>
-      </c>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>FSW programs</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
       <c r="Y14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z14" s="5"/>
+      <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26">
       <c r="B15" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
-        <v>HTC</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>26</v>
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>FSW programs</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1309,10 +1361,7 @@
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="8"/>
-      <c r="R15" s="11">
-        <f>R13/R14</f>
-        <v>1333333.3333333333</v>
-      </c>
+      <c r="R15" s="8"/>
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
       <c r="U15" s="8"/>
@@ -1326,11 +1375,11 @@
     </row>
     <row r="16" spans="1:26">
       <c r="B16" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$5</f>
-        <v>HTC</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>27</v>
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>FSW programs</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -1346,8 +1395,9 @@
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
-      <c r="R16" s="10">
-        <v>0.9</v>
+      <c r="R16" s="11">
+        <f>R12/R13</f>
+        <v>83333.333333333328</v>
       </c>
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
@@ -1360,230 +1410,258 @@
       </c>
       <c r="Z16" s="8"/>
     </row>
+    <row r="17" spans="2:26">
+      <c r="B17" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>FSW programs</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z17" s="8"/>
+    </row>
     <row r="18" spans="2:26">
       <c r="B18" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
-        <v>ART</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="9">
-        <f>20000000</f>
-        <v>20000000</v>
-      </c>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>FSW programs</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
       <c r="Y18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z18" s="6"/>
+      <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="2:26">
       <c r="B19" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
-        <v>ART</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="12">
-        <v>600</v>
-      </c>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
+        <f>'Populations &amp; programs'!$C$4</f>
+        <v>FSW programs</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
       <c r="Y19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z19" s="5"/>
-    </row>
-    <row r="20" spans="2:26">
-      <c r="B20" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
-        <v>ART</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="11">
-        <f>R18/R19</f>
-        <v>33333.333333333336</v>
-      </c>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z20" s="8"/>
+      <c r="Z19" s="8"/>
     </row>
     <row r="21" spans="2:26">
       <c r="B21" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$6</f>
-        <v>ART</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="10">
-        <v>1</v>
-      </c>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="8"/>
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>HTC</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="9">
+        <f>10000000</f>
+        <v>10000000</v>
+      </c>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="6"/>
       <c r="Y21" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z21" s="8"/>
+      <c r="Z21" s="6"/>
+    </row>
+    <row r="22" spans="2:26">
+      <c r="B22" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>HTC</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="13">
+        <v>7.5</v>
+      </c>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z22" s="5"/>
     </row>
     <row r="23" spans="2:26">
       <c r="B23" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
-        <v>Other</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="9">
-        <f>15000000</f>
-        <v>15000000</v>
-      </c>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
-      <c r="X23" s="6"/>
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>HTC</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
       <c r="Y23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z23" s="6"/>
+      <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="2:26">
       <c r="B24" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
-        <v>Other</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>HTC</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
       <c r="Y24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z24" s="5"/>
+      <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="2:26">
       <c r="B25" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
-        <v>Other</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>26</v>
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>HTC</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -1599,7 +1677,10 @@
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
+      <c r="R25" s="11">
+        <f>R21/R22</f>
+        <v>1333333.3333333333</v>
+      </c>
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
@@ -1613,11 +1694,11 @@
     </row>
     <row r="26" spans="2:26">
       <c r="B26" s="4" t="str">
-        <f>'Populations &amp; programs'!$C$7</f>
-        <v>Other</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>27</v>
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>HTC</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>29</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -1633,7 +1714,9 @@
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
+      <c r="R26" s="12">
+        <v>0.9</v>
+      </c>
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
       <c r="U26" s="8"/>
@@ -1644,6 +1727,631 @@
         <v>24</v>
       </c>
       <c r="Z26" s="8"/>
+    </row>
+    <row r="27" spans="2:26">
+      <c r="B27" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>HTC</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+      <c r="Y27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z27" s="8"/>
+    </row>
+    <row r="28" spans="2:26">
+      <c r="B28" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$5</f>
+        <v>HTC</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
+      <c r="X28" s="8"/>
+      <c r="Y28" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z28" s="8"/>
+    </row>
+    <row r="30" spans="2:26">
+      <c r="B30" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>ART</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="9">
+        <f>20000000</f>
+        <v>20000000</v>
+      </c>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+      <c r="Y30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z30" s="6"/>
+    </row>
+    <row r="31" spans="2:26">
+      <c r="B31" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>ART</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="13">
+        <v>600</v>
+      </c>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z31" s="5"/>
+    </row>
+    <row r="32" spans="2:26">
+      <c r="B32" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>ART</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8"/>
+      <c r="Y32" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z32" s="8"/>
+    </row>
+    <row r="33" spans="2:26">
+      <c r="B33" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>ART</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="8"/>
+      <c r="X33" s="8"/>
+      <c r="Y33" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z33" s="8"/>
+    </row>
+    <row r="34" spans="2:26">
+      <c r="B34" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>ART</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="11">
+        <f>R30/R31</f>
+        <v>33333.333333333336</v>
+      </c>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
+      <c r="Y34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z34" s="8"/>
+    </row>
+    <row r="35" spans="2:26">
+      <c r="B35" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>ART</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="12">
+        <v>1</v>
+      </c>
+      <c r="S35" s="8"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="8"/>
+      <c r="X35" s="8"/>
+      <c r="Y35" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z35" s="8"/>
+    </row>
+    <row r="36" spans="2:26">
+      <c r="B36" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>ART</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8"/>
+      <c r="W36" s="8"/>
+      <c r="X36" s="8"/>
+      <c r="Y36" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z36" s="8"/>
+    </row>
+    <row r="37" spans="2:26">
+      <c r="B37" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$6</f>
+        <v>ART</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z37" s="8"/>
+    </row>
+    <row r="39" spans="2:26">
+      <c r="B39" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="9">
+        <f>15000000</f>
+        <v>15000000</v>
+      </c>
+      <c r="S39" s="6"/>
+      <c r="T39" s="6"/>
+      <c r="U39" s="6"/>
+      <c r="V39" s="6"/>
+      <c r="W39" s="6"/>
+      <c r="X39" s="6"/>
+      <c r="Y39" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z39" s="6"/>
+    </row>
+    <row r="40" spans="2:26">
+      <c r="B40" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5"/>
+      <c r="V40" s="5"/>
+      <c r="W40" s="5"/>
+      <c r="X40" s="5"/>
+      <c r="Y40" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z40" s="5"/>
+    </row>
+    <row r="41" spans="2:26">
+      <c r="B41" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="8"/>
+      <c r="Y41" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z41" s="8"/>
+    </row>
+    <row r="42" spans="2:26">
+      <c r="B42" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="8"/>
+      <c r="W42" s="8"/>
+      <c r="X42" s="8"/>
+      <c r="Y42" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z42" s="8"/>
+    </row>
+    <row r="43" spans="2:26">
+      <c r="B43" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
+      <c r="V43" s="8"/>
+      <c r="W43" s="8"/>
+      <c r="X43" s="8"/>
+      <c r="Y43" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z43" s="8"/>
+    </row>
+    <row r="44" spans="2:26">
+      <c r="B44" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+      <c r="T44" s="8"/>
+      <c r="U44" s="8"/>
+      <c r="V44" s="8"/>
+      <c r="W44" s="8"/>
+      <c r="X44" s="8"/>
+      <c r="Y44" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z44" s="8"/>
+    </row>
+    <row r="45" spans="2:26">
+      <c r="B45" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+      <c r="T45" s="8"/>
+      <c r="U45" s="8"/>
+      <c r="V45" s="8"/>
+      <c r="W45" s="8"/>
+      <c r="X45" s="8"/>
+      <c r="Y45" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z45" s="8"/>
+    </row>
+    <row r="46" spans="2:26">
+      <c r="B46" s="4" t="str">
+        <f>'Populations &amp; programs'!$C$7</f>
+        <v>Other</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+      <c r="T46" s="8"/>
+      <c r="U46" s="8"/>
+      <c r="V46" s="8"/>
+      <c r="W46" s="8"/>
+      <c r="X46" s="8"/>
+      <c r="Y46" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z46" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>